<commit_message>
Added Rotation to the Player
</commit_message>
<xml_diff>
--- a/Arbeitsschritte.xlsx
+++ b/Arbeitsschritte.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vholt\Documents\Master\1.Semester\FortgeschritteneProgrammierung\Projekt\Project-Firefight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\HAW\Project-Firefight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B908B15-D3F8-403C-A537-E8206921CCC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5912C011-5B05-4550-BD12-C63672C54FF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D957DF76-B2F0-4DE9-BF90-64045C6D76CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D957DF76-B2F0-4DE9-BF90-64045C6D76CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Project Firefight</t>
   </si>
@@ -112,13 +112,19 @@
   </si>
   <si>
     <t>Tür mit der Axt einschlagen</t>
+  </si>
+  <si>
+    <t>In Bearbeitung</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +135,13 @@
     <font>
       <u/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -155,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -166,10 +179,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -487,28 +503,29 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -521,9 +538,11 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>24</v>
@@ -539,14 +558,14 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -554,7 +573,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
@@ -567,7 +586,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
@@ -582,7 +601,7 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
@@ -597,7 +616,9 @@
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
@@ -609,8 +630,10 @@
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
@@ -625,7 +648,7 @@
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
@@ -638,7 +661,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3"/>

</xml_diff>

<commit_message>
HydrantKey & Tutorial Shader
- Ready to use Model of the Hydrantkey
- First attempt for the Tutorial Outline Shader
</commit_message>
<xml_diff>
--- a/Arbeitsschritte.xlsx
+++ b/Arbeitsschritte.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\HAW\Project-Firefight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Master\1.Semester\FortgeschritteneProgrammierung\Projekt\Project-Firefight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737E1C94-8AFF-45B8-9078-21AA9A3CEFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10778DF4-A634-4571-A861-A7FE647CACF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{D957DF76-B2F0-4DE9-BF90-64045C6D76CA}"/>
+    <workbookView xWindow="1590" yWindow="3195" windowWidth="23400" windowHeight="12555" xr2:uid="{D957DF76-B2F0-4DE9-BF90-64045C6D76CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Project Firefight</t>
   </si>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB208B0-1560-4CD3-8CCC-413775C1C340}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,8 +749,12 @@
       <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>

</xml_diff>